<commit_message>
ERD & Excel modify
</commit_message>
<xml_diff>
--- a/4_테이블정의서_v1.0.xlsx
+++ b/4_테이블정의서_v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" tabRatio="696" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" tabRatio="696" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="표지" sheetId="2" r:id="rId1"/>
@@ -48,122 +48,122 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="144">
   <si>
     <t>전자약정 및 웹서비스 통합플랫폼 구축</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Version 0.1</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>프로젝트명</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>문 서 번 호</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>문서명</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>세 부 업 무</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>작 성 자</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>전태건</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>작 성 일</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>2020.05.25</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>구         분</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>설계</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>승 인 자</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>승 인 일</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>개정이력</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>버전</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>개정내용</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>개정일</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>작성자</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>승인자</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>1.0</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>최초작성</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>2020.05.25</t>
   </si>
   <si>
     <t>전태건</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
     <t>테이블정의서</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
     <t>NO</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>테이블명</t>
   </si>
   <si>
     <t>KIBOCMS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>테이블</t>
@@ -215,209 +215,206 @@
   </si>
   <si>
     <t>DB</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>구분</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>테이블 ID</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>테이블 명</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>테이블 목록</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>테이블 상세</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>문서번호:KIBO_ECWP_DS14</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>KIBO_ECWP_DS14</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Main</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>사용자</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>과목</t>
   </si>
   <si>
     <t>과목</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강과목</t>
   </si>
   <si>
     <t>수강과목</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>사용자 리스트를 관리한다.</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>과목 종류를 관리한다.</t>
   </si>
   <si>
     <t>과목 종류를 관리한다.</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>학생별 수강과목을 관리한다</t>
   </si>
   <si>
     <t>학생별 수강과목을 관리한다</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>User</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Subject</t>
   </si>
   <si>
     <t>Subject</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>TaskingClass</t>
-  </si>
-  <si>
-    <t>TaskingClass</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>User</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>사용자</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>sid</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>password</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>address</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>학번</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>이름</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>비밀번호</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>주소</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>전화번호</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>int</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>50</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>과목명</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강과목코드</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강과목명</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강학생학번</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강 시작시간</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>100</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>email</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>phone</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>email</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>create_dt</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>[sid,name]</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>20</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>50</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -434,183 +431,207 @@
       </rPr>
       <t>mail</t>
     </r>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>s_name</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>s_time</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>e_time</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>s_yoil</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강 요일</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>과목코드</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>s_code</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>datetime</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>[sCode,s_name]</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ts_sid</t>
-    <phoneticPr fontId="23" type="noConversion"/>
+    <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
     <t>ts_code</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ts_name</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>tsS_time</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>tsE_time</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ts_yoil</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ts_check</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>[ts_sid,ts_code]</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강과목시작시간</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강과목종료시간</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강 종시간</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강과목요일</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>출석체크</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_sid</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_subjectName</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>cS_time</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_yoil</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>cE_time</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_checkingTime</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_state</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>[c_sid,c_subjectName,c_checkingTime,c_state]</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>출석체크 한 학생의 과목 이름</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>출석체크 한 과목의 시작시간</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>출석체크 한 과목의 종료시간</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>출석체크 한 과목의 수강요일</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>출석체크 한 현재 시간</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 과목의 출석상태</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>출석체크 한 학생의 학번</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checking</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>출석체크</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목별 출석체크 상태를 관리한다.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checking</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>TakingClass</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ts_checkingTime </t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>수강체크상태</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>출석체크</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>c_sid</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
-    <t>c_subjectName</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>cS_time</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>c_yoil</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>cE_time</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>c_checkingTime</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>c_state</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>[c_sid,c_subjectName,c_checkingTime,c_state]</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>출석체크 한 학생의 과목 이름</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>출석체크 한 과목의 시작시간</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>출석체크 한 과목의 종료시간</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>출석체크 한 과목의 수강요일</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>출석체크 한 현재 시간</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당 과목의 출석상태</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>출석체크 한 학생의 학번</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>Checking</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>출석체크</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>과목별 출석체크 상태를 관리한다.</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>최신 수강신청 시간</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1161,13 +1182,16 @@
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1177,278 +1201,275 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="14">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="20" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="14" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="14">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="20" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="17" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="19" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="18" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="17" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="19" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="18" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="17" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="19" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="14" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="14" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="14" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="18" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="17" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="18" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="19" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="14" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -1506,7 +1527,7 @@
         <xdr:cNvPr id="3" name="그림 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1556,7 +1577,7 @@
         <xdr:cNvPr id="4" name="그림 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2157,16 +2178,16 @@
     <row r="4" spans="1:14" ht="31.5">
       <c r="B4" s="3"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" ht="32.25" thickBot="1">
       <c r="A5" s="5"/>
@@ -2176,13 +2197,13 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
     </row>
     <row r="6" spans="1:14" ht="32.25" thickTop="1">
       <c r="A6" s="33"/>
@@ -2194,11 +2215,11 @@
       <c r="D7" s="4"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="52" t="s">
+      <c r="J7" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
     </row>
     <row r="8" spans="1:14" ht="17.25">
       <c r="B8" s="3"/>
@@ -2254,52 +2275,52 @@
     </row>
     <row r="17" spans="1:12" ht="20.25">
       <c r="A17" s="10"/>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="55" t="s">
+      <c r="C17" s="63"/>
+      <c r="D17" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="57"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="66"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" ht="17.25">
       <c r="A18" s="10"/>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46" t="s">
+      <c r="C18" s="47"/>
+      <c r="D18" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
       <c r="G18" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="49"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="58"/>
     </row>
     <row r="19" spans="1:12" ht="17.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
       <c r="G19" s="15" t="s">
         <v>6</v>
       </c>
@@ -2309,22 +2330,22 @@
       <c r="I19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J19" s="58" t="s">
+      <c r="J19" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="59"/>
+      <c r="K19" s="50"/>
     </row>
     <row r="20" spans="1:12" ht="21" thickBot="1">
       <c r="A20" s="10"/>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62" t="s">
+      <c r="C20" s="52"/>
+      <c r="D20" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
       <c r="G20" s="16" t="s">
         <v>12</v>
       </c>
@@ -2332,8 +2353,8 @@
       <c r="I20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="55"/>
       <c r="L20" s="17"/>
     </row>
     <row r="21" spans="1:12" ht="17.25">
@@ -2364,12 +2385,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="H18:K18"/>
@@ -2378,8 +2393,14 @@
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="J20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2390,7 +2411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -2406,15 +2427,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B3" s="23" t="s">
@@ -2564,7 +2585,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59" right="0.7" top="1.1811023622047245" bottom="0.78740157480314965" header="0.6692913385826772" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
@@ -2576,7 +2597,7 @@
   <dimension ref="B2:G41"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2591,14 +2612,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="24.75" customHeight="1">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
     </row>
     <row r="3" spans="2:7" ht="16.5">
       <c r="B3" s="35" t="s">
@@ -2671,7 +2692,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="31" t="s">
         <v>59</v>
@@ -2691,13 +2712,13 @@
         <v>54</v>
       </c>
       <c r="E7" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="31" t="s">
         <v>138</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" customHeight="1">
@@ -2976,7 +2997,7 @@
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2984,10 +3005,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3005,49 +3026,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="72"/>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="74"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="84"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="68"/>
+      <c r="B2" s="70"/>
       <c r="C2" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="76"/>
+      <c r="E2" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="71"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="67" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="77"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" s="79"/>
+      <c r="I2" s="78"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="69" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="71"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="81"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="37" t="s">
@@ -3083,24 +3104,24 @@
         <v>1</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="40"/>
       <c r="F5" s="40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G5" s="38">
         <v>1</v>
       </c>
       <c r="H5" s="41"/>
       <c r="I5" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3108,26 +3129,26 @@
         <v>2</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" s="42">
         <v>1</v>
       </c>
       <c r="H6" s="41"/>
       <c r="I6" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3135,24 +3156,24 @@
         <v>3</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G7" s="42"/>
       <c r="H7" s="41"/>
       <c r="I7" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3160,22 +3181,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="41"/>
       <c r="G8" s="42"/>
       <c r="H8" s="41"/>
-      <c r="I8" s="84" t="s">
-        <v>99</v>
+      <c r="I8" s="45" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3183,22 +3204,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="41"/>
       <c r="G9" s="42"/>
       <c r="H9" s="41"/>
       <c r="I9" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3206,22 +3227,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F10" s="41"/>
       <c r="G10" s="42"/>
       <c r="H10" s="41"/>
       <c r="I10" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3229,17 +3250,17 @@
         <v>7</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="40"/>
-      <c r="F11" s="83" t="s">
-        <v>98</v>
+      <c r="F11" s="44" t="s">
+        <v>97</v>
       </c>
       <c r="G11" s="42"/>
       <c r="H11" s="41"/>
@@ -3251,80 +3272,80 @@
       <c r="A12" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="67" t="s">
+      <c r="C12" s="70"/>
+      <c r="D12" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="68"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="70"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="38">
         <v>1</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="80" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="82"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="72"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="74"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="84"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="68"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="75" t="s">
         <v>66</v>
       </c>
       <c r="D15" s="76"/>
-      <c r="E15" s="67" t="s">
+      <c r="E15" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="78" t="s">
+      <c r="F15" s="71"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="I15" s="79"/>
+      <c r="I15" s="78"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="69" t="s">
+      <c r="B16" s="70"/>
+      <c r="C16" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="71"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="81"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="37" t="s">
@@ -3360,16 +3381,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E18" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F18" s="40" t="s">
         <v>24</v>
@@ -3379,7 +3400,7 @@
       </c>
       <c r="H18" s="41"/>
       <c r="I18" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -3387,26 +3408,26 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F19" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" s="42">
         <v>1</v>
       </c>
       <c r="H19" s="41"/>
       <c r="I19" s="39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3414,20 +3435,20 @@
         <v>3</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E20" s="40"/>
       <c r="F20" s="43"/>
       <c r="G20" s="42"/>
       <c r="H20" s="41"/>
       <c r="I20" s="39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3435,20 +3456,20 @@
         <v>4</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" s="40"/>
       <c r="F21" s="43"/>
       <c r="G21" s="42"/>
       <c r="H21" s="41"/>
       <c r="I21" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -3456,102 +3477,102 @@
         <v>5</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F22" s="43"/>
       <c r="G22" s="42"/>
       <c r="H22" s="41"/>
-      <c r="I22" s="84" t="s">
-        <v>104</v>
+      <c r="I22" s="45" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="A23" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="67" t="s">
+      <c r="C23" s="70"/>
+      <c r="D23" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="68"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="70"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="38">
         <v>1</v>
       </c>
-      <c r="B24" s="80" t="s">
+      <c r="B24" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="82"/>
-      <c r="D24" s="80" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
-      <c r="I24" s="82"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="73"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="72"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="74"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="84"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="68"/>
+      <c r="B26" s="70"/>
       <c r="C26" s="75" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="D26" s="76"/>
-      <c r="E26" s="67" t="s">
+      <c r="E26" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="77"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="78" t="s">
+      <c r="F26" s="71"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="I26" s="79"/>
+      <c r="I26" s="78"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="67" t="s">
+      <c r="A27" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="69" t="s">
+      <c r="B27" s="70"/>
+      <c r="C27" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="71"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="81"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="37" t="s">
@@ -3587,16 +3608,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29" s="40" t="s">
         <v>24</v>
@@ -3606,7 +3627,7 @@
       </c>
       <c r="H29" s="41"/>
       <c r="I29" s="39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3614,16 +3635,16 @@
         <v>2</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D30" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F30" s="40" t="s">
         <v>24</v>
@@ -3633,7 +3654,7 @@
       </c>
       <c r="H30" s="41"/>
       <c r="I30" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3641,16 +3662,16 @@
         <v>3</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F31" s="40" t="s">
         <v>24</v>
@@ -3658,7 +3679,7 @@
       <c r="G31" s="42"/>
       <c r="H31" s="40"/>
       <c r="I31" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -3666,20 +3687,20 @@
         <v>4</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40"/>
       <c r="G32" s="42"/>
       <c r="H32" s="40"/>
       <c r="I32" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -3687,20 +3708,20 @@
         <v>5</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E33" s="40"/>
       <c r="F33" s="40"/>
       <c r="G33" s="42"/>
       <c r="H33" s="40"/>
       <c r="I33" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3708,22 +3729,22 @@
         <v>6</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D34" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E34" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F34" s="40"/>
       <c r="G34" s="42"/>
       <c r="H34" s="41"/>
       <c r="I34" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3731,346 +3752,376 @@
         <v>7</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E35" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F35" s="43"/>
       <c r="G35" s="42"/>
       <c r="H35" s="40"/>
       <c r="I35" s="39" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A36" s="37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="38">
+        <v>8</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" s="43"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="17.25" customHeight="1">
+      <c r="A37" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="67" t="s">
+      <c r="B37" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="68"/>
-      <c r="D36" s="67" t="s">
+      <c r="C37" s="70"/>
+      <c r="D37" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="68"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="38">
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="70"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="38">
         <v>1</v>
       </c>
-      <c r="B37" s="80" t="s">
+      <c r="B38" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="82"/>
-      <c r="D37" s="80" t="s">
-        <v>116</v>
-      </c>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="82"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="67" t="s">
+      <c r="C38" s="73"/>
+      <c r="D38" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="73"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="68"/>
-      <c r="C40" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="76"/>
-      <c r="E40" s="67" t="s">
+      <c r="B41" s="70"/>
+      <c r="C41" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" s="76"/>
+      <c r="E41" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="77"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="78" t="s">
-        <v>122</v>
-      </c>
-      <c r="I40" s="79"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="67" t="s">
+      <c r="F41" s="71"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="I41" s="78"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="68"/>
-      <c r="C41" s="69" t="s">
+      <c r="B42" s="70"/>
+      <c r="C42" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="71"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="37" t="s">
+      <c r="D42" s="80"/>
+      <c r="E42" s="80"/>
+      <c r="F42" s="80"/>
+      <c r="G42" s="80"/>
+      <c r="H42" s="80"/>
+      <c r="I42" s="81"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B43" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C43" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D43" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="37" t="s">
+      <c r="E43" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="37" t="s">
+      <c r="F43" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="G43" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="H42" s="37" t="s">
+      <c r="H43" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="I42" s="37" t="s">
+      <c r="I43" s="37" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="38">
-        <v>1</v>
-      </c>
-      <c r="B43" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="G43" s="42">
-        <v>1</v>
-      </c>
-      <c r="H43" s="41"/>
-      <c r="I43" s="39" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E44" s="40" t="s">
-        <v>83</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E44" s="40"/>
       <c r="F44" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="38">
+      <c r="G44" s="42">
         <v>1</v>
       </c>
       <c r="H44" s="41"/>
       <c r="I44" s="39" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E45" s="40"/>
+        <v>40</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>82</v>
+      </c>
       <c r="F45" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="42"/>
-      <c r="H45" s="40"/>
+      <c r="G45" s="38">
+        <v>1</v>
+      </c>
+      <c r="H45" s="41"/>
       <c r="I45" s="39" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E46" s="40"/>
       <c r="F46" s="40" t="s">
         <v>24</v>
       </c>
       <c r="G46" s="42"/>
-      <c r="H46" s="41"/>
+      <c r="H46" s="40"/>
       <c r="I46" s="39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E47" s="40" t="s">
-        <v>83</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E47" s="40"/>
       <c r="F47" s="40" t="s">
         <v>24</v>
       </c>
       <c r="G47" s="42"/>
       <c r="H47" s="41"/>
       <c r="I47" s="39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="38">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C48" s="39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48" s="40"/>
+        <v>40</v>
+      </c>
+      <c r="E48" s="40" t="s">
+        <v>82</v>
+      </c>
       <c r="F48" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="42">
-        <v>1</v>
-      </c>
+      <c r="G48" s="42"/>
       <c r="H48" s="41"/>
       <c r="I48" s="39" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="38">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C49" s="39" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="F49" s="43" t="s">
-        <v>82</v>
+        <v>106</v>
+      </c>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40" t="s">
+        <v>24</v>
       </c>
       <c r="G49" s="42">
         <v>1</v>
       </c>
-      <c r="H49" s="40"/>
+      <c r="H49" s="41"/>
       <c r="I49" s="39" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="38">
+        <v>7</v>
+      </c>
+      <c r="B50" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="F50" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="G50" s="42">
+        <v>1</v>
+      </c>
+      <c r="H50" s="40"/>
+      <c r="I50" s="39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="67" t="s">
+      <c r="B51" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="68"/>
-      <c r="D50" s="67" t="s">
+      <c r="C51" s="70"/>
+      <c r="D51" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="E50" s="77"/>
-      <c r="F50" s="77"/>
-      <c r="G50" s="77"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="68"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="38">
+      <c r="E51" s="71"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="71"/>
+      <c r="H51" s="71"/>
+      <c r="I51" s="70"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="38">
         <v>1</v>
       </c>
-      <c r="B51" s="80" t="s">
+      <c r="B52" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="82"/>
-      <c r="D51" s="80" t="s">
-        <v>130</v>
-      </c>
-      <c r="E51" s="81"/>
-      <c r="F51" s="81"/>
-      <c r="G51" s="81"/>
-      <c r="H51" s="81"/>
-      <c r="I51" s="82"/>
+      <c r="C52" s="73"/>
+      <c r="D52" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
+      <c r="H52" s="74"/>
+      <c r="I52" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:I50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:I51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:I36"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="D37:I37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:I38"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
@@ -4083,25 +4134,18 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:I23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:I51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:I52"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:I42"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -4117,12 +4161,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x010100F52CA7997D9787408D707D1BA85AF63C" ma:contentTypeVersion="8" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="32212bb438ab880763cb0b65f41616d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="33e2fe05-db15-4e39-8b35-7689cc124370" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="095822ebd38cad2f491effdf24e93c45" ns2:_="">
     <xsd:import namespace="33e2fe05-db15-4e39-8b35-7689cc124370"/>
@@ -4292,6 +4330,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{231FF65B-7903-47F7-83BC-11113BB10CAC}">
   <ds:schemaRefs>
@@ -4301,22 +4345,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{402C8E1C-F2E3-475F-8CB2-9D204C0820EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="bd5c06d0-0d80-408b-869c-235a7549c7d8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02EDB26F-541E-478C-956A-4287A559277D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4332,4 +4360,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{402C8E1C-F2E3-475F-8CB2-9D204C0820EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="bd5c06d0-0d80-408b-869c-235a7549c7d8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>